<commit_message>
Fix error handling of values
</commit_message>
<xml_diff>
--- a/bin/Sheets/BalanceSheets.xlsx
+++ b/bin/Sheets/BalanceSheets.xlsx
@@ -1195,23 +1195,23 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="18">
     <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="179" formatCode="0.0_ "/>
-    <numFmt numFmtId="180" formatCode="0.0_);[Red]\(0.0\)"/>
-    <numFmt numFmtId="181" formatCode="0.0%"/>
-    <numFmt numFmtId="182" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="183" formatCode="mmmm\ d\,\ yyyy"/>
+    <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="178" formatCode="0.0_);[Red]\(0.0\)"/>
+    <numFmt numFmtId="179" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="180" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="181" formatCode="0_ "/>
+    <numFmt numFmtId="182" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="183" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="184" formatCode="0%_);[Red]\(0%\)"/>
+    <numFmt numFmtId="185" formatCode="0.0_ "/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="186" formatCode="0.0%"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="184" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="185" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="186" formatCode="0_ "/>
     <numFmt numFmtId="187" formatCode="_-&quot;₱&quot;* #,##0.00_-;\-&quot;₱&quot;* #,##0.00_-;_-&quot;₱&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="188" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="189" formatCode="mmmm\ d\,\ yyyy"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="188" formatCode="0%_);[Red]\(0%\)"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="189" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
   <fonts count="54">
     <font>
@@ -1437,14 +1437,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Arial"/>
@@ -1468,13 +1460,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -1483,16 +1468,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1520,17 +1514,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1545,29 +1553,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1578,6 +1564,20 @@
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1747,7 +1747,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1759,31 +1777,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1795,7 +1789,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1813,31 +1813,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1849,7 +1855,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1861,13 +1867,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5428,16 +5428,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5457,26 +5457,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -5503,148 +5503,148 @@
   </borders>
   <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="184" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="182" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="185" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="34" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="183" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="39" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="304" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="304" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="48" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="46" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="303" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="303" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="27" borderId="299" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="44" fillId="30" borderId="302" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="187" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="39" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="301" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="299" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="29" borderId="300" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="29" borderId="300" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="27" borderId="300" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="47" fillId="30" borderId="300" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="188" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="302" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="184" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="301" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="298" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="298" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="298" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="298" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="25" borderId="297" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="25" borderId="297" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -5708,7 +5708,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5730,7 +5730,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -5746,7 +5746,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="20" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -5879,7 +5879,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="189" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -5895,13 +5895,13 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="7" fillId="5" borderId="51" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="7" fillId="5" borderId="51" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="7" fillId="5" borderId="53" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="7" fillId="5" borderId="53" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -5910,7 +5910,7 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="7" fillId="5" borderId="55" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="7" fillId="5" borderId="55" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -5925,49 +5925,49 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="7" fillId="5" borderId="58" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="7" fillId="5" borderId="58" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="7" fillId="6" borderId="59" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="7" fillId="6" borderId="59" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="8" fillId="7" borderId="59" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="8" fillId="7" borderId="59" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="7" fillId="5" borderId="59" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="7" fillId="5" borderId="59" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="8" fillId="5" borderId="59" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="8" fillId="5" borderId="59" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="8" fillId="5" borderId="60" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="8" fillId="5" borderId="60" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="7" fillId="5" borderId="62" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="7" fillId="5" borderId="62" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="7" fillId="5" borderId="63" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="7" fillId="5" borderId="63" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="7" fillId="5" borderId="64" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="7" fillId="5" borderId="64" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6000,7 +6000,7 @@
     <xf numFmtId="0" fontId="16" fillId="10" borderId="67" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="17" fillId="10" borderId="68" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="17" fillId="10" borderId="68" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="69" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -6018,7 +6018,7 @@
     <xf numFmtId="0" fontId="16" fillId="10" borderId="70" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="17" fillId="10" borderId="71" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="17" fillId="10" borderId="71" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="72" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -6027,7 +6027,7 @@
     <xf numFmtId="0" fontId="16" fillId="9" borderId="73" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="17" fillId="9" borderId="74" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="17" fillId="9" borderId="74" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="75" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -6036,7 +6036,7 @@
     <xf numFmtId="0" fontId="16" fillId="9" borderId="76" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="17" fillId="9" borderId="77" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="17" fillId="9" borderId="77" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -6048,7 +6048,7 @@
     <xf numFmtId="0" fontId="18" fillId="11" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="17" fillId="11" borderId="79" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="17" fillId="11" borderId="79" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="11" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -6075,7 +6075,7 @@
     <xf numFmtId="0" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="17" fillId="11" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="17" fillId="11" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="11" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -6114,10 +6114,10 @@
     <xf numFmtId="0" fontId="15" fillId="5" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="17" fillId="10" borderId="83" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="17" fillId="10" borderId="83" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="17" fillId="10" borderId="84" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="17" fillId="10" borderId="84" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="85" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -6126,28 +6126,28 @@
     <xf numFmtId="0" fontId="17" fillId="9" borderId="86" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="17" fillId="10" borderId="85" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="17" fillId="10" borderId="85" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="17" fillId="10" borderId="86" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="17" fillId="10" borderId="86" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="17" fillId="9" borderId="87" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="17" fillId="9" borderId="87" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="17" fillId="9" borderId="88" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="17" fillId="9" borderId="88" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="17" fillId="9" borderId="89" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="17" fillId="9" borderId="89" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="17" fillId="9" borderId="90" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="17" fillId="9" borderId="90" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="17" fillId="12" borderId="79" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="17" fillId="12" borderId="79" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="17" fillId="11" borderId="91" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="17" fillId="11" borderId="91" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="19" fillId="0" borderId="92" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -6171,10 +6171,10 @@
     <xf numFmtId="2" fontId="19" fillId="0" borderId="92" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="182" fontId="17" fillId="12" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="17" fillId="12" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="17" fillId="11" borderId="93" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="17" fillId="11" borderId="93" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="17" fillId="12" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -6205,17 +6205,17 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="3" fillId="5" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="3" fillId="5" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="186" fontId="21" fillId="5" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="21" fillId="5" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="1" fillId="13" borderId="97" xfId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="186" fontId="1" fillId="13" borderId="97" xfId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -6227,10 +6227,10 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="98" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -6242,7 +6242,7 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="99" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="189" fontId="1" fillId="13" borderId="97" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="179" fontId="1" fillId="13" borderId="97" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -6251,13 +6251,13 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="13" borderId="102" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="185" fontId="1" fillId="13" borderId="102" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -6278,7 +6278,7 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="177" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -6287,16 +6287,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="3" fillId="0" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="3" fillId="0" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="3" fillId="11" borderId="97" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="3" fillId="11" borderId="97" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -6308,7 +6308,7 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="107" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="11" borderId="108" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="3" fillId="11" borderId="108" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -6323,13 +6323,13 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="186" fontId="3" fillId="0" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="3" fillId="0" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="1" fillId="15" borderId="97" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="1" fillId="15" borderId="97" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -6413,19 +6413,19 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="21" fillId="15" borderId="97" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="21" fillId="15" borderId="97" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="99" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="126" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -6434,7 +6434,7 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="127" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="1" fillId="15" borderId="128" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="1" fillId="15" borderId="128" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="129" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -6443,29 +6443,29 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="185" fontId="1" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="130" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="5" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="185" fontId="3" fillId="5" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="5" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="185" fontId="3" fillId="5" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="17" borderId="97" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="185" fontId="1" fillId="17" borderId="97" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="185" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="185" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="131" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -6474,10 +6474,10 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="17" borderId="132" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="185" fontId="1" fillId="17" borderId="132" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="185" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -6860,50 +6860,50 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="181" xfId="10" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="206" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="206" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="207" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="207" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="208" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="208" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="209" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="209" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="208" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="208" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="209" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="209" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="210" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="210" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="211" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="211" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="8" borderId="206" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="8" borderId="206" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="8" borderId="207" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="8" borderId="207" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="8" borderId="208" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="8" borderId="208" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="8" borderId="209" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="8" borderId="209" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="8" borderId="210" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="8" borderId="210" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="8" borderId="211" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="8" borderId="211" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="10" applyFont="1"/>
@@ -6916,78 +6916,78 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="10" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="4" borderId="212" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="4" borderId="212" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="4" borderId="213" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="4" borderId="213" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="4" borderId="208" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="4" borderId="208" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="4" borderId="209" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="4" borderId="209" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="4" borderId="214" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="4" borderId="214" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="4" borderId="215" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="4" borderId="215" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="216" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="216" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="217" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="217" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="217" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="217" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="218" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="218" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="219" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="219" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="8" borderId="216" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="8" borderId="216" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="8" borderId="220" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="8" borderId="220" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="8" borderId="217" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="8" borderId="217" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="8" borderId="218" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="8" borderId="218" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="8" borderId="219" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="8" borderId="219" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="8" borderId="221" xfId="10" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="4" borderId="222" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="4" borderId="222" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="4" borderId="217" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="4" borderId="217" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="4" borderId="223" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="4" borderId="223" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="4" borderId="224" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="4" borderId="224" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -7000,124 +7000,124 @@
     <xf numFmtId="0" fontId="24" fillId="15" borderId="171" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="226" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="226" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="8" borderId="227" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="8" borderId="227" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="8" borderId="226" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="8" borderId="226" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="4" borderId="208" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="4" borderId="208" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="4" borderId="209" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="4" borderId="209" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="4" borderId="217" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="4" borderId="217" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="22" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="182" fontId="0" fillId="4" borderId="228" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="182" fontId="22" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="180" fontId="0" fillId="4" borderId="228" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="20" borderId="229" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="20" borderId="229" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="20" borderId="213" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="20" borderId="213" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="20" borderId="230" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="20" borderId="230" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="20" borderId="231" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="20" borderId="231" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="20" borderId="230" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="20" borderId="230" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="20" borderId="231" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="20" borderId="231" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="12" borderId="230" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="12" borderId="230" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="12" borderId="231" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="12" borderId="231" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="4" borderId="232" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="4" borderId="232" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="12" borderId="224" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="12" borderId="224" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="12" borderId="215" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="12" borderId="215" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="20" borderId="222" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="20" borderId="222" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="20" borderId="233" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="20" borderId="233" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="20" borderId="234" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="20" borderId="234" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="20" borderId="235" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="20" borderId="235" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="20" borderId="234" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="20" borderId="234" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="12" borderId="234" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="12" borderId="234" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="12" borderId="235" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="12" borderId="235" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="12" borderId="223" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="12" borderId="223" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="12" borderId="236" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="12" borderId="236" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="20" borderId="228" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="20" borderId="228" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="20" borderId="237" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="20" borderId="237" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="12" borderId="237" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="12" borderId="237" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="12" borderId="232" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="12" borderId="232" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="20" borderId="218" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="20" borderId="218" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="20" borderId="209" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="20" borderId="209" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="8" borderId="171" xfId="10" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="20" borderId="238" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="20" borderId="238" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="20" borderId="239" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="20" borderId="239" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="20" borderId="226" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="20" borderId="226" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="12" borderId="239" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="12" borderId="239" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="12" borderId="240" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="0" fillId="12" borderId="240" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="10" applyFill="1" applyBorder="1"/>
@@ -7170,56 +7170,56 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="13" borderId="243" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="210" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="13" borderId="243" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="210" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="211" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="211" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="11" borderId="246" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="11" borderId="246" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="15" borderId="144" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="15" borderId="144" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="15" borderId="145" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="15" borderId="145" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="219" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="219" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="248" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="248" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="249" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="249" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="11" borderId="250" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="11" borderId="250" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="11" borderId="251" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="11" borderId="251" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="15" borderId="171" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="15" borderId="171" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="252" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="252" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="13" borderId="253" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="254" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="255" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="13" borderId="253" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="254" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="255" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="11" borderId="256" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="11" borderId="256" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="19" borderId="144" xfId="10" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7278,23 +7278,23 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="207" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="207" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="249" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="249" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="264" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="264" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="10" borderId="209" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="10" borderId="209" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="21" borderId="259" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="182" fontId="0" fillId="22" borderId="265" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="21" borderId="259" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="0" fillId="22" borderId="265" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="19" borderId="171" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -7305,44 +7305,44 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="216" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="216" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="220" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="220" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="218" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="218" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="252" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="252" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="248" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="248" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="266" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="266" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="267" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="267" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="10" borderId="217" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="10" borderId="217" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="10" borderId="218" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="10" borderId="218" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="22" borderId="268" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="22" borderId="268" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="22" borderId="269" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="22" borderId="269" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="183" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -7359,7 +7359,7 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="227" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="227" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -7370,14 +7370,14 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="272" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="226" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="226" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="272" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="255" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="255" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -7385,21 +7385,21 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="13" borderId="256" xfId="10" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="182" fontId="0" fillId="8" borderId="273" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="180" fontId="0" fillId="8" borderId="273" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="10" borderId="226" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="10" borderId="226" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="272" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="8" fillId="5" borderId="272" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="188" fontId="8" fillId="5" borderId="272" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="21" borderId="274" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="182" fontId="0" fillId="22" borderId="275" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="21" borderId="274" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="0" fillId="22" borderId="275" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="276" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -7411,10 +7411,10 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="7" fillId="6" borderId="59" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="188" fontId="7" fillId="6" borderId="59" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="6" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="176" fontId="7" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="187" fontId="7" fillId="6" borderId="59" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -7423,7 +7423,7 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="8" fillId="5" borderId="0" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="188" fontId="8" fillId="5" borderId="0" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="187" fontId="7" fillId="5" borderId="272" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -7484,62 +7484,62 @@
     <xf numFmtId="0" fontId="29" fillId="22" borderId="282" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="22" borderId="283" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="22" borderId="283" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="22" borderId="284" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="22" borderId="284" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="23" borderId="280" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="23" borderId="280" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="22" borderId="285" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="22" borderId="285" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="23" borderId="265" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="23" borderId="265" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="22" borderId="286" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="22" borderId="286" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="22" borderId="287" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="22" borderId="287" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="22" borderId="288" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="22" borderId="288" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="23" borderId="289" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="23" borderId="289" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="22" borderId="290" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="22" borderId="290" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="23" borderId="291" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="23" borderId="291" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="23" borderId="268" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="23" borderId="268" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="22" borderId="292" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="22" borderId="292" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="22" borderId="293" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="22" borderId="293" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="23" borderId="294" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="23" borderId="294" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="22" borderId="295" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="22" borderId="295" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="296" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="296" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="55">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Currency_simple" xfId="1"/>
-    <cellStyle name="Currency 2" xfId="2"/>
-    <cellStyle name="Comma 3" xfId="3"/>
-    <cellStyle name="Comma 2" xfId="4"/>
+    <cellStyle name="Comma 2" xfId="1"/>
+    <cellStyle name="Comma 3" xfId="2"/>
+    <cellStyle name="Currency 2" xfId="3"/>
+    <cellStyle name="Currency_simple" xfId="4"/>
     <cellStyle name="60% - Accent6" xfId="5" builtinId="52"/>
     <cellStyle name="40% - Accent6" xfId="6" builtinId="51"/>
     <cellStyle name="60% - Accent5" xfId="7" builtinId="48"/>
@@ -9598,7 +9598,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -21759,7 +21759,7 @@
   <sheetPr/>
   <dimension ref="C1:AV56"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A23" workbookViewId="0">
       <selection activeCell="AC34" sqref="AC34:AH34"/>
     </sheetView>
   </sheetViews>
@@ -27445,10 +27445,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F98"/>
+  <dimension ref="A1:F99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+      <selection activeCell="E99" sqref="E99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="5"/>
@@ -27476,7 +27476,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" ht="13.5" spans="1:6">
       <c r="A2" s="187" t="s">
         <v>199</v>
       </c>
@@ -28364,7 +28364,7 @@
       <c r="E58" s="223"/>
       <c r="F58" s="255"/>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" ht="13.5" spans="1:6">
       <c r="A59" s="224"/>
       <c r="B59" s="225" t="s">
         <v>255</v>
@@ -28383,7 +28383,7 @@
       </c>
       <c r="F59" s="256"/>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" ht="13.5" spans="1:6">
       <c r="A60" s="184"/>
       <c r="B60" s="184"/>
       <c r="C60" s="184"/>
@@ -28730,7 +28730,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" ht="13.5" spans="1:6">
       <c r="A83" s="266"/>
       <c r="B83" s="267" t="s">
         <v>278</v>
@@ -28757,7 +28757,7 @@
       <c r="E84" s="184"/>
       <c r="F84" s="247"/>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" ht="13.5" spans="1:6">
       <c r="A85" s="269" t="s">
         <v>279</v>
       </c>
@@ -28890,7 +28890,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" ht="13.5" spans="1:6">
       <c r="A93" s="279"/>
       <c r="B93" s="280" t="s">
         <v>288</v>
@@ -28909,7 +28909,7 @@
       </c>
       <c r="F93" s="299"/>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" ht="14.25" spans="1:6">
       <c r="A94" s="184"/>
       <c r="B94" s="184"/>
       <c r="C94" s="282"/>
@@ -28917,7 +28917,7 @@
       <c r="E94" s="282"/>
       <c r="F94" s="247"/>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" ht="13.5" spans="1:6">
       <c r="A95" s="269" t="s">
         <v>289</v>
       </c>
@@ -28971,25 +28971,26 @@
         <v>283</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" ht="13.5" spans="1:6">
       <c r="A98" s="279"/>
       <c r="B98" s="280" t="s">
         <v>292</v>
       </c>
       <c r="C98" s="281">
-        <f>C96/C97</f>
+        <f>IFERROR(C96/C97,"")</f>
         <v>0.0210610606747644</v>
       </c>
       <c r="D98" s="281">
-        <f>D96/D97</f>
+        <f>IFERROR(D96/D97,"")</f>
         <v>0.0403175950675635</v>
       </c>
       <c r="E98" s="281">
-        <f>E96/E97</f>
+        <f>IFERROR(E96/E97,"")</f>
         <v>0.0933321940578929</v>
       </c>
       <c r="F98" s="299"/>
     </row>
+    <row r="99" ht="13.5"/>
   </sheetData>
   <mergeCells count="32">
     <mergeCell ref="A2:A37"/>

</xml_diff>